<commit_message>
Update to database, documentation and sql creation scripts
</commit_message>
<xml_diff>
--- a/documentation/business_data.xlsx
+++ b/documentation/business_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="497">
   <si>
     <t>Online Car Repair</t>
   </si>
@@ -1212,6 +1212,9 @@
     <t>Post_codes</t>
   </si>
   <si>
+    <t>Customer Ids</t>
+  </si>
+  <si>
     <t>TACT-19</t>
   </si>
   <si>
@@ -1227,6 +1230,9 @@
     <t>Post_code</t>
   </si>
   <si>
+    <t>User ID</t>
+  </si>
+  <si>
     <t>TACT-21</t>
   </si>
   <si>
@@ -1236,6 +1242,9 @@
     <t>PST-01</t>
   </si>
   <si>
+    <t>USR-01</t>
+  </si>
+  <si>
     <t>TACT-22</t>
   </si>
   <si>
@@ -1248,6 +1257,9 @@
     <t>PST-02</t>
   </si>
   <si>
+    <t>USR-02</t>
+  </si>
+  <si>
     <t>TACT-23</t>
   </si>
   <si>
@@ -1260,6 +1272,9 @@
     <t>PST-03</t>
   </si>
   <si>
+    <t>USR-03</t>
+  </si>
+  <si>
     <t>TACT-24</t>
   </si>
   <si>
@@ -1272,6 +1287,9 @@
     <t>PST-04</t>
   </si>
   <si>
+    <t>USR-04</t>
+  </si>
+  <si>
     <t>TACT-25</t>
   </si>
   <si>
@@ -1284,36 +1302,54 @@
     <t>PST-05</t>
   </si>
   <si>
+    <t>USR-05</t>
+  </si>
+  <si>
     <t>TACT-26</t>
   </si>
   <si>
     <t>PST-06</t>
   </si>
   <si>
+    <t>USR-06</t>
+  </si>
+  <si>
     <t>TACT-27</t>
   </si>
   <si>
     <t>PST-07</t>
   </si>
   <si>
+    <t>USR-07</t>
+  </si>
+  <si>
     <t>TACT-28</t>
   </si>
   <si>
     <t>PST-08</t>
   </si>
   <si>
+    <t>USR-08</t>
+  </si>
+  <si>
     <t>TACT-29</t>
   </si>
   <si>
     <t>PST-09</t>
   </si>
   <si>
+    <t>USR-09</t>
+  </si>
+  <si>
     <t>TACT-30</t>
   </si>
   <si>
     <t>PST-10</t>
   </si>
   <si>
+    <t>USR-10</t>
+  </si>
+  <si>
     <t>TACT-31</t>
   </si>
   <si>
@@ -1350,6 +1386,9 @@
     <t>LS6 2AB</t>
   </si>
   <si>
+    <t>Staff Ids</t>
+  </si>
+  <si>
     <t>TACT-35</t>
   </si>
   <si>
@@ -1368,6 +1407,12 @@
     <t>BS8 3JD</t>
   </si>
   <si>
+    <t>staff_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
     <t>TACT-37</t>
   </si>
   <si>
@@ -1377,9 +1422,51 @@
     <t>BN2 1RD</t>
   </si>
   <si>
+    <t>STF-01</t>
+  </si>
+  <si>
+    <t>USR-11</t>
+  </si>
+  <si>
+    <t>STF-02</t>
+  </si>
+  <si>
+    <t>USR-12</t>
+  </si>
+  <si>
+    <t>STF-03</t>
+  </si>
+  <si>
+    <t>USR-13</t>
+  </si>
+  <si>
+    <t>STF-04</t>
+  </si>
+  <si>
+    <t>USR-14</t>
+  </si>
+  <si>
+    <t>STF-05</t>
+  </si>
+  <si>
+    <t>USR-15</t>
+  </si>
+  <si>
+    <t>STF-06</t>
+  </si>
+  <si>
+    <t>USR-16</t>
+  </si>
+  <si>
     <t>User table</t>
   </si>
   <si>
+    <t>STF-07</t>
+  </si>
+  <si>
+    <t>USR-17</t>
+  </si>
+  <si>
     <t>User_id</t>
   </si>
   <si>
@@ -1407,40 +1494,13 @@
     <t>Access_Code</t>
   </si>
   <si>
-    <t>USR-01</t>
-  </si>
-  <si>
-    <t>USR-02</t>
-  </si>
-  <si>
-    <t>USR-03</t>
-  </si>
-  <si>
-    <t>USR-04</t>
-  </si>
-  <si>
-    <t>USR-05</t>
-  </si>
-  <si>
-    <t>USR-06</t>
-  </si>
-  <si>
-    <t>USR-07</t>
-  </si>
-  <si>
-    <t>USR-08</t>
-  </si>
-  <si>
-    <t>USR-09</t>
-  </si>
-  <si>
-    <t>USR-10</t>
-  </si>
-  <si>
-    <t>USR-11</t>
-  </si>
-  <si>
-    <t>STF-01</t>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>account_creation_date</t>
   </si>
   <si>
     <t>12 Baker Street</t>
@@ -1452,60 +1512,30 @@
     <t>Mechanic</t>
   </si>
   <si>
-    <t>USR-12</t>
-  </si>
-  <si>
-    <t>STF-02</t>
-  </si>
-  <si>
     <t>45 Oakwood Drive</t>
   </si>
   <si>
     <t>07941 994567</t>
   </si>
   <si>
-    <t>USR-13</t>
-  </si>
-  <si>
-    <t>STF-03</t>
-  </si>
-  <si>
     <t>88 Kingsway Road</t>
   </si>
   <si>
     <t>07722 556688</t>
   </si>
   <si>
-    <t>USR-14</t>
-  </si>
-  <si>
-    <t>STF-04</t>
-  </si>
-  <si>
     <t>3 Rose Hill Crescent</t>
   </si>
   <si>
     <t>07400 123456</t>
   </si>
   <si>
-    <t>USR-15</t>
-  </si>
-  <si>
-    <t>STF-05</t>
-  </si>
-  <si>
     <t>101 Castle Street</t>
   </si>
   <si>
     <t>020 7946 0123</t>
   </si>
   <si>
-    <t>USR-16</t>
-  </si>
-  <si>
-    <t>STF-06</t>
-  </si>
-  <si>
     <t>Sue Bridges</t>
   </si>
   <si>
@@ -1519,12 +1549,6 @@
   </si>
   <si>
     <t>FRNT-01</t>
-  </si>
-  <si>
-    <t>USR-17</t>
-  </si>
-  <si>
-    <t>STF-07</t>
   </si>
   <si>
     <t>Alex Towns</t>
@@ -1546,7 +1570,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1580,6 +1604,17 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1776,7 +1811,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1836,6 +1871,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1916,6 +1954,9 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="15" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -7815,7 +7856,7 @@
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -7982,45 +8023,45 @@
       <c r="Z7" s="25"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="30" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="M8" s="27" t="s">
+      <c r="M8" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="N8" s="27" t="s">
+      <c r="N8" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="O8" s="29" t="s">
+      <c r="O8" s="30" t="s">
         <v>134</v>
       </c>
       <c r="P8" s="25"/>
@@ -8036,45 +8077,45 @@
       <c r="Z8" s="25"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="33" t="s">
         <v>135</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="34" t="s">
         <v>46</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="L9" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="O9" s="33" t="s">
+      <c r="O9" s="34" t="s">
         <v>145</v>
       </c>
       <c r="P9" s="25"/>
@@ -8090,45 +8131,45 @@
       <c r="Z9" s="25"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="33" t="s">
         <v>151</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="34" t="s">
         <v>46</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="L10" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="N10" s="32" t="s">
+      <c r="N10" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="O10" s="33" t="s">
+      <c r="O10" s="34" t="s">
         <v>158</v>
       </c>
       <c r="P10" s="25"/>
@@ -8144,45 +8185,45 @@
       <c r="Z10" s="25"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="33" t="s">
         <v>159</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="34" t="s">
         <v>31</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
-      <c r="I11" s="35" t="s">
+      <c r="I11" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="L11" s="36" t="s">
+      <c r="L11" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="M11" s="36" t="s">
+      <c r="M11" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="N11" s="36" t="s">
+      <c r="N11" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="O11" s="37" t="s">
+      <c r="O11" s="38" t="s">
         <v>173</v>
       </c>
       <c r="P11" s="25"/>
@@ -8198,22 +8239,22 @@
       <c r="Z11" s="25"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="33" t="s">
         <v>151</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="34" t="s">
         <v>46</v>
       </c>
       <c r="G12" s="25"/>
@@ -8238,22 +8279,22 @@
       <c r="Z12" s="25"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="33" t="s">
         <v>174</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="34" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="25"/>
@@ -8278,22 +8319,22 @@
       <c r="Z13" s="25"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="33" t="s">
         <v>180</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="34" t="s">
         <v>46</v>
       </c>
       <c r="G14" s="25"/>
@@ -8318,22 +8359,22 @@
       <c r="Z14" s="25"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="33" t="s">
         <v>186</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="34" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="25"/>
@@ -8358,22 +8399,22 @@
       <c r="Z15" s="25"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="33" t="s">
         <v>192</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="34" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="25"/>
@@ -8398,22 +8439,22 @@
       <c r="Z16" s="25"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="39" t="s">
         <v>242</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="37" t="s">
         <v>243</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="40" t="s">
         <v>46</v>
       </c>
       <c r="G17" s="25"/>
@@ -8638,50 +8679,50 @@
       <c r="Z23" s="25"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="35" t="s">
         <v>249</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="H24" s="32" t="s">
+      <c r="H24" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="I24" s="40">
+      <c r="I24" s="41">
         <v>45936.0</v>
       </c>
-      <c r="J24" s="40" t="s">
+      <c r="J24" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K24" s="40" t="s">
+      <c r="K24" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L24" s="41" t="s">
+      <c r="L24" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M24" s="41">
+      <c r="M24" s="42">
         <v>180.0</v>
       </c>
-      <c r="N24" s="41">
+      <c r="N24" s="42">
         <f t="shared" ref="N24:N33" si="1">M24*0.2</f>
         <v>36</v>
       </c>
-      <c r="O24" s="42">
+      <c r="O24" s="43">
         <f t="shared" ref="O24:O33" si="2">M24+N24</f>
         <v>216</v>
       </c>
@@ -8698,50 +8739,50 @@
       <c r="Z24" s="25"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="H25" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="41">
         <v>45931.0</v>
       </c>
-      <c r="J25" s="40" t="s">
+      <c r="J25" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="K25" s="40" t="s">
+      <c r="K25" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="L25" s="41" t="s">
+      <c r="L25" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M25" s="41">
+      <c r="M25" s="42">
         <v>80.0</v>
       </c>
-      <c r="N25" s="41">
+      <c r="N25" s="42">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="O25" s="42">
+      <c r="O25" s="43">
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
@@ -8758,50 +8799,50 @@
       <c r="Z25" s="25"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="F26" s="32" t="s">
+      <c r="F26" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="H26" s="32" t="s">
+      <c r="H26" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="I26" s="40">
+      <c r="I26" s="41">
         <v>45945.0</v>
       </c>
-      <c r="J26" s="40" t="s">
+      <c r="J26" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="40" t="s">
+      <c r="K26" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L26" s="41" t="s">
+      <c r="L26" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M26" s="41">
+      <c r="M26" s="42">
         <v>80.0</v>
       </c>
-      <c r="N26" s="41">
+      <c r="N26" s="42">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="O26" s="42">
+      <c r="O26" s="43">
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
@@ -8818,50 +8859,50 @@
       <c r="Z26" s="25"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="32" t="s">
+      <c r="G27" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="41">
         <v>45940.0</v>
       </c>
-      <c r="J27" s="40" t="s">
+      <c r="J27" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K27" s="40" t="s">
+      <c r="K27" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="41" t="s">
+      <c r="L27" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M27" s="41">
+      <c r="M27" s="42">
         <v>180.0</v>
       </c>
-      <c r="N27" s="41">
+      <c r="N27" s="42">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="O27" s="42">
+      <c r="O27" s="43">
         <f t="shared" si="2"/>
         <v>216</v>
       </c>
@@ -8878,50 +8919,50 @@
       <c r="Z27" s="25"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="D28" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E28" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="F28" s="32" t="s">
+      <c r="F28" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="32" t="s">
+      <c r="H28" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="I28" s="40">
+      <c r="I28" s="41">
         <v>45933.0</v>
       </c>
-      <c r="J28" s="40" t="s">
+      <c r="J28" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="40" t="s">
+      <c r="K28" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="L28" s="41" t="s">
+      <c r="L28" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M28" s="41">
+      <c r="M28" s="42">
         <v>120.0</v>
       </c>
-      <c r="N28" s="41">
+      <c r="N28" s="42">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="O28" s="42">
+      <c r="O28" s="43">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
@@ -8938,50 +8979,50 @@
       <c r="Z28" s="25"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="F29" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H29" s="33" t="s">
         <v>264</v>
       </c>
-      <c r="I29" s="40">
+      <c r="I29" s="41">
         <v>45948.0</v>
       </c>
-      <c r="J29" s="40" t="s">
+      <c r="J29" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="40" t="s">
+      <c r="K29" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L29" s="41" t="s">
+      <c r="L29" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M29" s="41">
+      <c r="M29" s="42">
         <v>450.0</v>
       </c>
-      <c r="N29" s="41">
+      <c r="N29" s="42">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="O29" s="42">
+      <c r="O29" s="43">
         <f t="shared" si="2"/>
         <v>540</v>
       </c>
@@ -8998,50 +9039,50 @@
       <c r="Z29" s="25"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="35" t="s">
         <v>265</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="H30" s="32" t="s">
+      <c r="H30" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="I30" s="40">
+      <c r="I30" s="41">
         <v>45939.0</v>
       </c>
-      <c r="J30" s="40" t="s">
+      <c r="J30" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K30" s="40" t="s">
+      <c r="K30" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="L30" s="41" t="s">
+      <c r="L30" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M30" s="41">
+      <c r="M30" s="42">
         <v>120.0</v>
       </c>
-      <c r="N30" s="41">
+      <c r="N30" s="42">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="O30" s="42">
+      <c r="O30" s="43">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
@@ -9058,50 +9099,50 @@
       <c r="Z30" s="25"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="F31" s="32" t="s">
+      <c r="F31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="H31" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="I31" s="40">
+      <c r="I31" s="41">
         <v>45943.0</v>
       </c>
-      <c r="J31" s="40" t="s">
+      <c r="J31" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="K31" s="40" t="s">
+      <c r="K31" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="L31" s="41" t="s">
+      <c r="L31" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M31" s="41">
+      <c r="M31" s="42">
         <v>175.0</v>
       </c>
-      <c r="N31" s="41">
+      <c r="N31" s="42">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="O31" s="42">
+      <c r="O31" s="43">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
@@ -9118,50 +9159,50 @@
       <c r="Z31" s="25"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="35" t="s">
         <v>267</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="33" t="s">
         <v>241</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E32" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="32" t="s">
+      <c r="G32" s="33" t="s">
         <v>268</v>
       </c>
-      <c r="H32" s="32" t="s">
+      <c r="H32" s="33" t="s">
         <v>264</v>
       </c>
-      <c r="I32" s="40">
+      <c r="I32" s="41">
         <v>45928.0</v>
       </c>
-      <c r="J32" s="40" t="s">
+      <c r="J32" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="K32" s="40" t="s">
+      <c r="K32" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L32" s="41" t="s">
+      <c r="L32" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="M32" s="41">
+      <c r="M32" s="42">
         <v>85.0</v>
       </c>
-      <c r="N32" s="41">
+      <c r="N32" s="42">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="O32" s="42">
+      <c r="O32" s="43">
         <f t="shared" si="2"/>
         <v>102</v>
       </c>
@@ -9178,50 +9219,50 @@
       <c r="Z32" s="25"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="37" t="s">
         <v>243</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="E33" s="36" t="s">
+      <c r="E33" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="F33" s="36" t="s">
+      <c r="F33" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="G33" s="36" t="s">
+      <c r="G33" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="H33" s="36" t="s">
+      <c r="H33" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="I33" s="43">
+      <c r="I33" s="44">
         <v>45946.0</v>
       </c>
-      <c r="J33" s="43" t="s">
+      <c r="J33" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="43" t="s">
+      <c r="K33" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="L33" s="43" t="s">
+      <c r="L33" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="M33" s="44">
+      <c r="M33" s="45">
         <v>140.0</v>
       </c>
-      <c r="N33" s="44">
+      <c r="N33" s="45">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="O33" s="45">
+      <c r="O33" s="46">
         <f t="shared" si="2"/>
         <v>168</v>
       </c>
@@ -9242,7 +9283,7 @@
       <c r="B34" s="25"/>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
-      <c r="E34" s="32"/>
+      <c r="E34" s="33"/>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
@@ -9326,7 +9367,7 @@
       <c r="B37" s="25"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
-      <c r="E37" s="32"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
       <c r="H37" s="25"/>
@@ -9522,19 +9563,19 @@
       <c r="Z42" s="25"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="32" t="s">
         <v>283</v>
       </c>
       <c r="B43" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="33" t="s">
         <v>216</v>
       </c>
       <c r="D43" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="E43" s="46">
+      <c r="E43" s="47">
         <v>1.0</v>
       </c>
       <c r="F43" s="25"/>
@@ -9554,7 +9595,7 @@
       <c r="L43" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="M43" s="32" t="s">
+      <c r="M43" s="33" t="s">
         <v>29</v>
       </c>
       <c r="N43" s="9" t="s">
@@ -9576,19 +9617,19 @@
       <c r="Z43" s="25"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="32" t="s">
         <v>290</v>
       </c>
       <c r="B44" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="33" t="s">
         <v>216</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="E44" s="46">
+      <c r="E44" s="47">
         <v>1.0</v>
       </c>
       <c r="F44" s="25"/>
@@ -9608,7 +9649,7 @@
       <c r="L44" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="M44" s="32" t="s">
+      <c r="M44" s="33" t="s">
         <v>44</v>
       </c>
       <c r="N44" s="9" t="s">
@@ -9630,19 +9671,19 @@
       <c r="Z44" s="25"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="32" t="s">
         <v>297</v>
       </c>
       <c r="B45" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="33" t="s">
         <v>216</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="E45" s="46">
+      <c r="E45" s="47">
         <v>1.0</v>
       </c>
       <c r="F45" s="25"/>
@@ -9662,7 +9703,7 @@
       <c r="L45" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="M45" s="32" t="s">
+      <c r="M45" s="33" t="s">
         <v>66</v>
       </c>
       <c r="N45" s="9" t="s">
@@ -9684,19 +9725,19 @@
       <c r="Z45" s="25"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="32" t="s">
         <v>303</v>
       </c>
       <c r="B46" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="C46" s="32" t="s">
+      <c r="C46" s="33" t="s">
         <v>216</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="E46" s="46">
+      <c r="E46" s="47">
         <v>4.0</v>
       </c>
       <c r="F46" s="25"/>
@@ -9716,7 +9757,7 @@
       <c r="L46" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="M46" s="36" t="s">
+      <c r="M46" s="37" t="s">
         <v>78</v>
       </c>
       <c r="N46" s="14" t="s">
@@ -9738,19 +9779,19 @@
       <c r="Z46" s="25"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="32" t="s">
         <v>309</v>
       </c>
       <c r="B47" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="C47" s="32" t="s">
+      <c r="C47" s="33" t="s">
         <v>220</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="E47" s="46">
+      <c r="E47" s="47">
         <v>1.0</v>
       </c>
       <c r="F47" s="25"/>
@@ -9784,19 +9825,19 @@
       <c r="Z47" s="25"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="32" t="s">
         <v>315</v>
       </c>
       <c r="B48" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="C48" s="32" t="s">
+      <c r="C48" s="33" t="s">
         <v>220</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="E48" s="46">
+      <c r="E48" s="47">
         <v>2.0</v>
       </c>
       <c r="F48" s="25"/>
@@ -9830,19 +9871,19 @@
       <c r="Z48" s="25"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="32" t="s">
         <v>321</v>
       </c>
       <c r="B49" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="33" t="s">
         <v>220</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="E49" s="46">
+      <c r="E49" s="47">
         <v>1.0</v>
       </c>
       <c r="F49" s="25"/>
@@ -9876,19 +9917,19 @@
       <c r="Z49" s="25"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="32" t="s">
         <v>327</v>
       </c>
       <c r="B50" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="33" t="s">
         <v>224</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="E50" s="46">
+      <c r="E50" s="47">
         <v>1.0</v>
       </c>
       <c r="F50" s="25"/>
@@ -9924,19 +9965,19 @@
       <c r="Z50" s="25"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="32" t="s">
         <v>333</v>
       </c>
       <c r="B51" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="C51" s="32" t="s">
+      <c r="C51" s="33" t="s">
         <v>224</v>
       </c>
       <c r="D51" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="E51" s="46">
+      <c r="E51" s="47">
         <v>2.0</v>
       </c>
       <c r="F51" s="25"/>
@@ -9970,19 +10011,19 @@
       <c r="Z51" s="25"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="32" t="s">
         <v>337</v>
       </c>
       <c r="B52" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="C52" s="32" t="s">
+      <c r="C52" s="33" t="s">
         <v>224</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="E52" s="46">
+      <c r="E52" s="47">
         <v>1.0</v>
       </c>
       <c r="F52" s="25"/>
@@ -9999,19 +10040,19 @@
         <v>340</v>
       </c>
       <c r="K52" s="25"/>
-      <c r="L52" s="47" t="s">
+      <c r="L52" s="48" t="s">
         <v>341</v>
       </c>
-      <c r="M52" s="48" t="s">
+      <c r="M52" s="49" t="s">
         <v>342</v>
       </c>
-      <c r="N52" s="48" t="s">
+      <c r="N52" s="49" t="s">
         <v>343</v>
       </c>
-      <c r="O52" s="48" t="s">
+      <c r="O52" s="49" t="s">
         <v>344</v>
       </c>
-      <c r="P52" s="49" t="s">
+      <c r="P52" s="50" t="s">
         <v>345</v>
       </c>
       <c r="Q52" s="25"/>
@@ -10026,19 +10067,19 @@
       <c r="Z52" s="25"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="32" t="s">
         <v>346</v>
       </c>
       <c r="B53" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="C53" s="32" t="s">
+      <c r="C53" s="33" t="s">
         <v>228</v>
       </c>
       <c r="D53" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="E53" s="46">
+      <c r="E53" s="47">
         <v>1.0</v>
       </c>
       <c r="F53" s="25"/>
@@ -10055,19 +10096,19 @@
         <v>349</v>
       </c>
       <c r="K53" s="25"/>
-      <c r="L53" s="50" t="s">
+      <c r="L53" s="51" t="s">
         <v>350</v>
       </c>
-      <c r="M53" s="27" t="s">
+      <c r="M53" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="N53" s="51">
+      <c r="N53" s="52">
         <v>1.0</v>
       </c>
-      <c r="O53" s="51" t="s">
+      <c r="O53" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="P53" s="52" t="s">
+      <c r="P53" s="53" t="s">
         <v>351</v>
       </c>
       <c r="Q53" s="25"/>
@@ -10082,19 +10123,19 @@
       <c r="Z53" s="25"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="32" t="s">
         <v>352</v>
       </c>
       <c r="B54" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="C54" s="32" t="s">
+      <c r="C54" s="33" t="s">
         <v>228</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="E54" s="46">
+      <c r="E54" s="47">
         <v>1.0</v>
       </c>
       <c r="F54" s="25"/>
@@ -10114,7 +10155,7 @@
       <c r="L54" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="M54" s="32" t="s">
+      <c r="M54" s="33" t="s">
         <v>233</v>
       </c>
       <c r="N54" s="9">
@@ -10138,19 +10179,19 @@
       <c r="Z54" s="25"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="32" t="s">
         <v>359</v>
       </c>
       <c r="B55" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="C55" s="32" t="s">
+      <c r="C55" s="33" t="s">
         <v>228</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="E55" s="46">
+      <c r="E55" s="47">
         <v>1.0</v>
       </c>
       <c r="F55" s="25"/>
@@ -10170,7 +10211,7 @@
       <c r="L55" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="M55" s="36" t="s">
+      <c r="M55" s="37" t="s">
         <v>243</v>
       </c>
       <c r="N55" s="14">
@@ -10194,19 +10235,19 @@
       <c r="Z55" s="25"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="32" t="s">
         <v>366</v>
       </c>
       <c r="B56" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="C56" s="32" t="s">
+      <c r="C56" s="33" t="s">
         <v>228</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="E56" s="46">
+      <c r="E56" s="47">
         <v>4.0</v>
       </c>
       <c r="F56" s="25"/>
@@ -10240,19 +10281,19 @@
       <c r="Z56" s="25"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="32" t="s">
         <v>371</v>
       </c>
       <c r="B57" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="C57" s="32" t="s">
+      <c r="C57" s="33" t="s">
         <v>232</v>
       </c>
       <c r="D57" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="E57" s="46">
+      <c r="E57" s="47">
         <v>1.0</v>
       </c>
       <c r="F57" s="25"/>
@@ -10286,19 +10327,19 @@
       <c r="Z57" s="25"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="32" t="s">
         <v>376</v>
       </c>
       <c r="B58" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="C58" s="32" t="s">
+      <c r="C58" s="33" t="s">
         <v>232</v>
       </c>
       <c r="D58" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="E58" s="46">
+      <c r="E58" s="47">
         <v>6.0</v>
       </c>
       <c r="F58" s="25"/>
@@ -10324,19 +10365,19 @@
       <c r="Z58" s="25"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="32" t="s">
         <v>377</v>
       </c>
       <c r="B59" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="C59" s="32" t="s">
+      <c r="C59" s="33" t="s">
         <v>232</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="E59" s="46">
+      <c r="E59" s="47">
         <v>1.0</v>
       </c>
       <c r="F59" s="25"/>
@@ -10362,19 +10403,19 @@
       <c r="Z59" s="25"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="32" t="s">
         <v>378</v>
       </c>
       <c r="B60" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C60" s="32" t="s">
+      <c r="C60" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="D60" s="32" t="s">
+      <c r="D60" s="33" t="s">
         <v>284</v>
       </c>
-      <c r="E60" s="46">
+      <c r="E60" s="47">
         <v>1.0</v>
       </c>
       <c r="F60" s="25"/>
@@ -10389,8 +10430,10 @@
       <c r="M60" s="3"/>
       <c r="N60" s="25"/>
       <c r="O60" s="25"/>
-      <c r="P60" s="25"/>
-      <c r="Q60" s="25"/>
+      <c r="P60" s="54" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q60" s="3"/>
       <c r="R60" s="25"/>
       <c r="S60" s="25"/>
       <c r="T60" s="25"/>
@@ -10402,24 +10445,24 @@
       <c r="Z60" s="25"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="31" t="s">
-        <v>380</v>
+      <c r="A61" s="32" t="s">
+        <v>381</v>
       </c>
       <c r="B61" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="D61" s="32" t="s">
+      <c r="D61" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="E61" s="46">
+      <c r="E61" s="47">
         <v>1.0</v>
       </c>
       <c r="F61" s="25"/>
       <c r="G61" s="20" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="25"/>
@@ -10442,19 +10485,19 @@
       <c r="Z61" s="25"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="31" t="s">
-        <v>382</v>
+      <c r="A62" s="32" t="s">
+        <v>383</v>
       </c>
       <c r="B62" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C62" s="32" t="s">
+      <c r="C62" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="D62" s="32" t="s">
+      <c r="D62" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="E62" s="46">
+      <c r="E62" s="47">
         <v>1.0</v>
       </c>
       <c r="F62" s="25"/>
@@ -10463,19 +10506,20 @@
       <c r="I62" s="25"/>
       <c r="J62" s="25"/>
       <c r="K62" s="25"/>
-      <c r="L62" s="53" t="s">
-        <v>383</v>
-      </c>
-      <c r="M62" s="54" t="s">
+      <c r="L62" s="55" t="s">
         <v>384</v>
       </c>
-      <c r="N62" s="25" t="str">
-        <f>L62&amp;","&amp;M62</f>
-        <v>Post_code_id,Post_code</v>
-      </c>
+      <c r="M62" s="56" t="s">
+        <v>385</v>
+      </c>
+      <c r="N62" s="25"/>
       <c r="O62" s="25"/>
-      <c r="P62" s="25"/>
-      <c r="Q62" s="25"/>
+      <c r="P62" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q62" s="26" t="s">
+        <v>386</v>
+      </c>
       <c r="R62" s="25"/>
       <c r="S62" s="25"/>
       <c r="T62" s="25"/>
@@ -10487,24 +10531,24 @@
       <c r="Z62" s="25"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="31" t="s">
-        <v>385</v>
+      <c r="A63" s="32" t="s">
+        <v>387</v>
       </c>
       <c r="B63" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C63" s="32" t="s">
+      <c r="C63" s="33" t="s">
         <v>234</v>
       </c>
       <c r="D63" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="E63" s="46">
+      <c r="E63" s="47">
         <v>4.0</v>
       </c>
       <c r="F63" s="25"/>
       <c r="G63" s="4" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>279</v>
@@ -10512,20 +10556,21 @@
       <c r="I63" s="25"/>
       <c r="J63" s="25"/>
       <c r="K63" s="25"/>
-      <c r="L63" s="55" t="s">
-        <v>387</v>
-      </c>
-      <c r="M63" s="56" t="s">
+      <c r="L63" s="57" t="s">
+        <v>389</v>
+      </c>
+      <c r="M63" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="N63" s="25" t="str">
-        <f t="shared" ref="N63:N83" si="3">CONCATENATE("('",L63,"',")&amp;CONCATENATE("'",M63,"'),")</f>
-        <v>('PST-01','CB2 1TN'),</v>
-      </c>
+      <c r="N63" s="25"/>
       <c r="O63" s="25"/>
-      <c r="P63" s="25"/>
-      <c r="Q63" s="25"/>
-      <c r="R63" s="25"/>
+      <c r="P63" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q63" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="R63" s="26"/>
       <c r="S63" s="25"/>
       <c r="T63" s="25"/>
       <c r="U63" s="25"/>
@@ -10536,45 +10581,46 @@
       <c r="Z63" s="25"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="31" t="s">
-        <v>388</v>
+      <c r="A64" s="32" t="s">
+        <v>391</v>
       </c>
       <c r="B64" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="33" t="s">
         <v>234</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="E64" s="46">
+      <c r="E64" s="47">
         <v>2.0</v>
       </c>
       <c r="F64" s="25"/>
-      <c r="G64" s="50" t="s">
-        <v>389</v>
-      </c>
-      <c r="H64" s="29" t="s">
-        <v>390</v>
+      <c r="G64" s="51" t="s">
+        <v>392</v>
+      </c>
+      <c r="H64" s="30" t="s">
+        <v>393</v>
       </c>
       <c r="I64" s="25"/>
       <c r="J64" s="25"/>
       <c r="K64" s="25"/>
-      <c r="L64" s="57" t="s">
-        <v>391</v>
-      </c>
-      <c r="M64" s="58" t="s">
+      <c r="L64" s="59" t="s">
+        <v>394</v>
+      </c>
+      <c r="M64" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="N64" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-02','SW3 4RY'),</v>
-      </c>
+      <c r="N64" s="25"/>
       <c r="O64" s="25"/>
-      <c r="P64" s="25"/>
-      <c r="Q64" s="25"/>
-      <c r="R64" s="25"/>
+      <c r="P64" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q64" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="R64" s="26"/>
       <c r="S64" s="25"/>
       <c r="T64" s="25"/>
       <c r="U64" s="25"/>
@@ -10585,45 +10631,46 @@
       <c r="Z64" s="25"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="31" t="s">
-        <v>392</v>
+      <c r="A65" s="32" t="s">
+        <v>396</v>
       </c>
       <c r="B65" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="33" t="s">
         <v>234</v>
       </c>
       <c r="D65" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="E65" s="46">
+      <c r="E65" s="47">
         <v>6.0</v>
       </c>
       <c r="F65" s="25"/>
       <c r="G65" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="H65" s="33" t="s">
-        <v>394</v>
+        <v>397</v>
+      </c>
+      <c r="H65" s="34" t="s">
+        <v>398</v>
       </c>
       <c r="I65" s="25"/>
       <c r="J65" s="25"/>
       <c r="K65" s="25"/>
-      <c r="L65" s="57" t="s">
-        <v>395</v>
-      </c>
-      <c r="M65" s="58" t="s">
+      <c r="L65" s="59" t="s">
+        <v>399</v>
+      </c>
+      <c r="M65" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="N65" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-03','M20 6WE'),</v>
-      </c>
+      <c r="N65" s="25"/>
       <c r="O65" s="25"/>
-      <c r="P65" s="25"/>
-      <c r="Q65" s="25"/>
-      <c r="R65" s="25"/>
+      <c r="P65" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q65" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="R65" s="26"/>
       <c r="S65" s="25"/>
       <c r="T65" s="25"/>
       <c r="U65" s="25"/>
@@ -10634,45 +10681,46 @@
       <c r="Z65" s="25"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="31" t="s">
-        <v>396</v>
+      <c r="A66" s="32" t="s">
+        <v>401</v>
       </c>
       <c r="B66" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C66" s="32" t="s">
+      <c r="C66" s="33" t="s">
         <v>234</v>
       </c>
       <c r="D66" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="E66" s="46">
+      <c r="E66" s="47">
         <v>1.0</v>
       </c>
       <c r="F66" s="25"/>
       <c r="G66" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="H66" s="33" t="s">
-        <v>398</v>
+        <v>402</v>
+      </c>
+      <c r="H66" s="34" t="s">
+        <v>403</v>
       </c>
       <c r="I66" s="25"/>
       <c r="J66" s="25"/>
       <c r="K66" s="25"/>
-      <c r="L66" s="57" t="s">
-        <v>399</v>
-      </c>
-      <c r="M66" s="58" t="s">
+      <c r="L66" s="59" t="s">
+        <v>404</v>
+      </c>
+      <c r="M66" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="N66" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-04','B15 2TH'),</v>
-      </c>
+      <c r="N66" s="25"/>
       <c r="O66" s="25"/>
-      <c r="P66" s="25"/>
-      <c r="Q66" s="25"/>
-      <c r="R66" s="25"/>
+      <c r="P66" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q66" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="R66" s="26"/>
       <c r="S66" s="25"/>
       <c r="T66" s="25"/>
       <c r="U66" s="25"/>
@@ -10683,45 +10731,46 @@
       <c r="Z66" s="25"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="31" t="s">
-        <v>400</v>
+      <c r="A67" s="32" t="s">
+        <v>406</v>
       </c>
       <c r="B67" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="C67" s="32" t="s">
+      <c r="C67" s="33" t="s">
         <v>234</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="E67" s="46">
+      <c r="E67" s="47">
         <v>1.0</v>
       </c>
       <c r="F67" s="25"/>
       <c r="G67" s="13" t="s">
-        <v>401</v>
-      </c>
-      <c r="H67" s="37" t="s">
-        <v>402</v>
+        <v>407</v>
+      </c>
+      <c r="H67" s="38" t="s">
+        <v>408</v>
       </c>
       <c r="I67" s="25"/>
       <c r="J67" s="25"/>
       <c r="K67" s="25"/>
-      <c r="L67" s="57" t="s">
-        <v>403</v>
-      </c>
-      <c r="M67" s="58" t="s">
+      <c r="L67" s="59" t="s">
+        <v>409</v>
+      </c>
+      <c r="M67" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="N67" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-05','LS1 4HT'),</v>
-      </c>
+      <c r="N67" s="25"/>
       <c r="O67" s="25"/>
-      <c r="P67" s="25"/>
-      <c r="Q67" s="25"/>
-      <c r="R67" s="25"/>
+      <c r="P67" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q67" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="R67" s="26"/>
       <c r="S67" s="25"/>
       <c r="T67" s="25"/>
       <c r="U67" s="25"/>
@@ -10732,19 +10781,19 @@
       <c r="Z67" s="25"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="31" t="s">
-        <v>404</v>
+      <c r="A68" s="32" t="s">
+        <v>411</v>
       </c>
       <c r="B68" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="C68" s="32" t="s">
+      <c r="C68" s="33" t="s">
         <v>236</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="E68" s="46">
+      <c r="E68" s="47">
         <v>1.0</v>
       </c>
       <c r="F68" s="25"/>
@@ -10753,20 +10802,21 @@
       <c r="I68" s="25"/>
       <c r="J68" s="25"/>
       <c r="K68" s="25"/>
-      <c r="L68" s="57" t="s">
-        <v>405</v>
-      </c>
-      <c r="M68" s="58" t="s">
+      <c r="L68" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="M68" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="N68" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-06','G1 3DX'),</v>
-      </c>
+      <c r="N68" s="25"/>
       <c r="O68" s="25"/>
-      <c r="P68" s="25"/>
-      <c r="Q68" s="25"/>
-      <c r="R68" s="25"/>
+      <c r="P68" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q68" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="R68" s="26"/>
       <c r="S68" s="25"/>
       <c r="T68" s="25"/>
       <c r="U68" s="25"/>
@@ -10777,19 +10827,19 @@
       <c r="Z68" s="25"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="31" t="s">
-        <v>406</v>
+      <c r="A69" s="32" t="s">
+        <v>414</v>
       </c>
       <c r="B69" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="C69" s="32" t="s">
+      <c r="C69" s="33" t="s">
         <v>236</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="E69" s="46">
+      <c r="E69" s="47">
         <v>6.0</v>
       </c>
       <c r="F69" s="25"/>
@@ -10798,20 +10848,21 @@
       <c r="I69" s="25"/>
       <c r="J69" s="25"/>
       <c r="K69" s="25"/>
-      <c r="L69" s="57" t="s">
-        <v>407</v>
-      </c>
-      <c r="M69" s="58" t="s">
+      <c r="L69" s="59" t="s">
+        <v>415</v>
+      </c>
+      <c r="M69" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="N69" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-07','BS3 5RW'),</v>
-      </c>
+      <c r="N69" s="25"/>
       <c r="O69" s="25"/>
-      <c r="P69" s="25"/>
-      <c r="Q69" s="25"/>
-      <c r="R69" s="25"/>
+      <c r="P69" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q69" s="32" t="s">
+        <v>416</v>
+      </c>
+      <c r="R69" s="26"/>
       <c r="S69" s="25"/>
       <c r="T69" s="25"/>
       <c r="U69" s="25"/>
@@ -10822,19 +10873,19 @@
       <c r="Z69" s="25"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="31" t="s">
-        <v>408</v>
+      <c r="A70" s="32" t="s">
+        <v>417</v>
       </c>
       <c r="B70" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="C70" s="32" t="s">
+      <c r="C70" s="33" t="s">
         <v>236</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="E70" s="46">
+      <c r="E70" s="47">
         <v>1.0</v>
       </c>
       <c r="F70" s="25"/>
@@ -10843,20 +10894,21 @@
       <c r="I70" s="25"/>
       <c r="J70" s="25"/>
       <c r="K70" s="25"/>
-      <c r="L70" s="57" t="s">
-        <v>409</v>
-      </c>
-      <c r="M70" s="58" t="s">
+      <c r="L70" s="59" t="s">
+        <v>418</v>
+      </c>
+      <c r="M70" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="N70" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-08','NG5 2BL'),</v>
-      </c>
+      <c r="N70" s="25"/>
       <c r="O70" s="25"/>
-      <c r="P70" s="25"/>
-      <c r="Q70" s="25"/>
-      <c r="R70" s="25"/>
+      <c r="P70" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q70" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="R70" s="26"/>
       <c r="S70" s="25"/>
       <c r="T70" s="25"/>
       <c r="U70" s="25"/>
@@ -10867,8 +10919,8 @@
       <c r="Z70" s="25"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="31" t="s">
-        <v>410</v>
+      <c r="A71" s="32" t="s">
+        <v>420</v>
       </c>
       <c r="B71" s="25" t="s">
         <v>266</v>
@@ -10879,7 +10931,7 @@
       <c r="D71" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="E71" s="46">
+      <c r="E71" s="47">
         <v>1.0</v>
       </c>
       <c r="F71" s="25"/>
@@ -10888,20 +10940,21 @@
       <c r="I71" s="25"/>
       <c r="J71" s="25"/>
       <c r="K71" s="25"/>
-      <c r="L71" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="M71" s="58" t="s">
+      <c r="L71" s="59" t="s">
+        <v>421</v>
+      </c>
+      <c r="M71" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="N71" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-09','L1 2SR'),</v>
-      </c>
+      <c r="N71" s="25"/>
       <c r="O71" s="25"/>
-      <c r="P71" s="25"/>
-      <c r="Q71" s="25"/>
-      <c r="R71" s="25"/>
+      <c r="P71" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q71" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="R71" s="26"/>
       <c r="S71" s="25"/>
       <c r="T71" s="25"/>
       <c r="U71" s="25"/>
@@ -10912,8 +10965,8 @@
       <c r="Z71" s="25"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="31" t="s">
-        <v>412</v>
+      <c r="A72" s="32" t="s">
+        <v>423</v>
       </c>
       <c r="B72" s="25" t="s">
         <v>266</v>
@@ -10924,7 +10977,7 @@
       <c r="D72" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="E72" s="46">
+      <c r="E72" s="47">
         <v>4.0</v>
       </c>
       <c r="F72" s="25"/>
@@ -10933,20 +10986,21 @@
       <c r="I72" s="25"/>
       <c r="J72" s="25"/>
       <c r="K72" s="25"/>
-      <c r="L72" s="57" t="s">
-        <v>413</v>
-      </c>
-      <c r="M72" s="58" t="s">
+      <c r="L72" s="59" t="s">
+        <v>424</v>
+      </c>
+      <c r="M72" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="N72" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-10','S10 1AA'),</v>
-      </c>
+      <c r="N72" s="25"/>
       <c r="O72" s="25"/>
-      <c r="P72" s="25"/>
-      <c r="Q72" s="25"/>
-      <c r="R72" s="25"/>
+      <c r="P72" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q72" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="R72" s="26"/>
       <c r="S72" s="25"/>
       <c r="T72" s="25"/>
       <c r="U72" s="25"/>
@@ -10957,8 +11011,8 @@
       <c r="Z72" s="25"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="31" t="s">
-        <v>414</v>
+      <c r="A73" s="32" t="s">
+        <v>426</v>
       </c>
       <c r="B73" s="25" t="s">
         <v>266</v>
@@ -10969,7 +11023,7 @@
       <c r="D73" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="E73" s="46">
+      <c r="E73" s="47">
         <v>2.0</v>
       </c>
       <c r="F73" s="25"/>
@@ -10978,16 +11032,13 @@
       <c r="I73" s="25"/>
       <c r="J73" s="25"/>
       <c r="K73" s="25"/>
-      <c r="L73" s="57" t="s">
-        <v>415</v>
-      </c>
-      <c r="M73" s="58" t="s">
-        <v>416</v>
-      </c>
-      <c r="N73" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-11','NW1 6XE'),</v>
-      </c>
+      <c r="L73" s="59" t="s">
+        <v>427</v>
+      </c>
+      <c r="M73" s="60" t="s">
+        <v>428</v>
+      </c>
+      <c r="N73" s="25"/>
       <c r="O73" s="25"/>
       <c r="P73" s="25"/>
       <c r="Q73" s="25"/>
@@ -11002,8 +11053,8 @@
       <c r="Z73" s="25"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="31" t="s">
-        <v>417</v>
+      <c r="A74" s="32" t="s">
+        <v>429</v>
       </c>
       <c r="B74" s="25" t="s">
         <v>266</v>
@@ -11014,7 +11065,7 @@
       <c r="D74" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="E74" s="46">
+      <c r="E74" s="47">
         <v>1.0</v>
       </c>
       <c r="F74" s="25"/>
@@ -11023,16 +11074,13 @@
       <c r="I74" s="25"/>
       <c r="J74" s="25"/>
       <c r="K74" s="25"/>
-      <c r="L74" s="57" t="s">
-        <v>418</v>
-      </c>
-      <c r="M74" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="N74" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-12','M14 5GH'),</v>
-      </c>
+      <c r="L74" s="59" t="s">
+        <v>430</v>
+      </c>
+      <c r="M74" s="60" t="s">
+        <v>431</v>
+      </c>
+      <c r="N74" s="25"/>
       <c r="O74" s="25"/>
       <c r="P74" s="25"/>
       <c r="Q74" s="25"/>
@@ -11047,8 +11095,8 @@
       <c r="Z74" s="25"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="31" t="s">
-        <v>420</v>
+      <c r="A75" s="32" t="s">
+        <v>432</v>
       </c>
       <c r="B75" s="25" t="s">
         <v>267</v>
@@ -11059,7 +11107,7 @@
       <c r="D75" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="E75" s="46">
+      <c r="E75" s="47">
         <v>2.0</v>
       </c>
       <c r="F75" s="25"/>
@@ -11068,16 +11116,13 @@
       <c r="I75" s="25"/>
       <c r="J75" s="25"/>
       <c r="K75" s="25"/>
-      <c r="L75" s="57" t="s">
-        <v>421</v>
-      </c>
-      <c r="M75" s="58" t="s">
-        <v>422</v>
-      </c>
-      <c r="N75" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-13','B15 2TT'),</v>
-      </c>
+      <c r="L75" s="59" t="s">
+        <v>433</v>
+      </c>
+      <c r="M75" s="60" t="s">
+        <v>434</v>
+      </c>
+      <c r="N75" s="25"/>
       <c r="O75" s="25"/>
       <c r="P75" s="25"/>
       <c r="Q75" s="25"/>
@@ -11092,8 +11137,8 @@
       <c r="Z75" s="25"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="31" t="s">
-        <v>423</v>
+      <c r="A76" s="32" t="s">
+        <v>435</v>
       </c>
       <c r="B76" s="25" t="s">
         <v>267</v>
@@ -11104,7 +11149,7 @@
       <c r="D76" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="E76" s="46">
+      <c r="E76" s="47">
         <v>1.0</v>
       </c>
       <c r="F76" s="25"/>
@@ -11113,19 +11158,18 @@
       <c r="I76" s="25"/>
       <c r="J76" s="25"/>
       <c r="K76" s="25"/>
-      <c r="L76" s="57" t="s">
-        <v>424</v>
-      </c>
-      <c r="M76" s="58" t="s">
-        <v>425</v>
-      </c>
-      <c r="N76" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-14','LS6 2AB'),</v>
-      </c>
+      <c r="L76" s="59" t="s">
+        <v>436</v>
+      </c>
+      <c r="M76" s="60" t="s">
+        <v>437</v>
+      </c>
+      <c r="N76" s="25"/>
       <c r="O76" s="25"/>
-      <c r="P76" s="25"/>
-      <c r="Q76" s="25"/>
+      <c r="P76" s="54" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q76" s="3"/>
       <c r="R76" s="25"/>
       <c r="S76" s="25"/>
       <c r="T76" s="25"/>
@@ -11137,8 +11181,8 @@
       <c r="Z76" s="25"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="31" t="s">
-        <v>426</v>
+      <c r="A77" s="32" t="s">
+        <v>439</v>
       </c>
       <c r="B77" s="25" t="s">
         <v>269</v>
@@ -11149,7 +11193,7 @@
       <c r="D77" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="E77" s="46">
+      <c r="E77" s="47">
         <v>1.0</v>
       </c>
       <c r="F77" s="25"/>
@@ -11158,16 +11202,13 @@
       <c r="I77" s="25"/>
       <c r="J77" s="25"/>
       <c r="K77" s="25"/>
-      <c r="L77" s="57" t="s">
-        <v>427</v>
-      </c>
-      <c r="M77" s="58" t="s">
-        <v>428</v>
-      </c>
-      <c r="N77" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-15','EH1 2NG'),</v>
-      </c>
+      <c r="L77" s="59" t="s">
+        <v>440</v>
+      </c>
+      <c r="M77" s="60" t="s">
+        <v>441</v>
+      </c>
+      <c r="N77" s="25"/>
       <c r="O77" s="25"/>
       <c r="P77" s="25"/>
       <c r="Q77" s="25"/>
@@ -11182,8 +11223,8 @@
       <c r="Z77" s="25"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="31" t="s">
-        <v>429</v>
+      <c r="A78" s="32" t="s">
+        <v>442</v>
       </c>
       <c r="B78" s="25" t="s">
         <v>269</v>
@@ -11194,7 +11235,7 @@
       <c r="D78" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="E78" s="46">
+      <c r="E78" s="47">
         <v>6.0</v>
       </c>
       <c r="F78" s="25"/>
@@ -11203,19 +11244,20 @@
       <c r="I78" s="25"/>
       <c r="J78" s="25"/>
       <c r="K78" s="25"/>
-      <c r="L78" s="57" t="s">
-        <v>430</v>
-      </c>
-      <c r="M78" s="58" t="s">
-        <v>431</v>
-      </c>
-      <c r="N78" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-16','BS8 3JD'),</v>
-      </c>
+      <c r="L78" s="59" t="s">
+        <v>443</v>
+      </c>
+      <c r="M78" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="N78" s="25"/>
       <c r="O78" s="25"/>
-      <c r="P78" s="25"/>
-      <c r="Q78" s="25"/>
+      <c r="P78" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q78" s="26" t="s">
+        <v>446</v>
+      </c>
       <c r="R78" s="25"/>
       <c r="S78" s="25"/>
       <c r="T78" s="25"/>
@@ -11227,19 +11269,19 @@
       <c r="Z78" s="25"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="38" t="s">
-        <v>432</v>
-      </c>
-      <c r="B79" s="59" t="s">
+      <c r="A79" s="39" t="s">
+        <v>447</v>
+      </c>
+      <c r="B79" s="61" t="s">
         <v>269</v>
       </c>
-      <c r="C79" s="59" t="s">
+      <c r="C79" s="61" t="s">
         <v>242</v>
       </c>
-      <c r="D79" s="59" t="s">
+      <c r="D79" s="61" t="s">
         <v>323</v>
       </c>
-      <c r="E79" s="60">
+      <c r="E79" s="62">
         <v>1.0</v>
       </c>
       <c r="F79" s="25"/>
@@ -11248,19 +11290,20 @@
       <c r="I79" s="25"/>
       <c r="J79" s="25"/>
       <c r="K79" s="25"/>
-      <c r="L79" s="57" t="s">
-        <v>433</v>
-      </c>
-      <c r="M79" s="58" t="s">
-        <v>434</v>
-      </c>
-      <c r="N79" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-17','BN2 1RD'),</v>
-      </c>
+      <c r="L79" s="59" t="s">
+        <v>448</v>
+      </c>
+      <c r="M79" s="60" t="s">
+        <v>449</v>
+      </c>
+      <c r="N79" s="25"/>
       <c r="O79" s="25"/>
-      <c r="P79" s="25"/>
-      <c r="Q79" s="25"/>
+      <c r="P79" s="25" t="s">
+        <v>450</v>
+      </c>
+      <c r="Q79" s="32" t="s">
+        <v>451</v>
+      </c>
       <c r="R79" s="25"/>
       <c r="S79" s="25"/>
       <c r="T79" s="25"/>
@@ -11283,19 +11326,20 @@
       <c r="I80" s="25"/>
       <c r="J80" s="25"/>
       <c r="K80" s="25"/>
-      <c r="L80" s="57" t="s">
+      <c r="L80" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="M80" s="58" t="s">
+      <c r="M80" s="60" t="s">
         <v>199</v>
       </c>
-      <c r="N80" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-18','M19 1AQ'),</v>
-      </c>
+      <c r="N80" s="25"/>
       <c r="O80" s="25"/>
-      <c r="P80" s="25"/>
-      <c r="Q80" s="25"/>
+      <c r="P80" s="25" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q80" s="32" t="s">
+        <v>453</v>
+      </c>
       <c r="R80" s="25"/>
       <c r="S80" s="25"/>
       <c r="T80" s="25"/>
@@ -11318,19 +11362,20 @@
       <c r="I81" s="25"/>
       <c r="J81" s="25"/>
       <c r="K81" s="25"/>
-      <c r="L81" s="57" t="s">
+      <c r="L81" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="M81" s="58" t="s">
+      <c r="M81" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="N81" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-19','MK9 1BB'),</v>
-      </c>
+      <c r="N81" s="25"/>
       <c r="O81" s="25"/>
-      <c r="P81" s="25"/>
-      <c r="Q81" s="25"/>
+      <c r="P81" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q81" s="32" t="s">
+        <v>455</v>
+      </c>
       <c r="R81" s="25"/>
       <c r="S81" s="25"/>
       <c r="T81" s="25"/>
@@ -11353,19 +11398,20 @@
       <c r="I82" s="25"/>
       <c r="J82" s="25"/>
       <c r="K82" s="25"/>
-      <c r="L82" s="57" t="s">
+      <c r="L82" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="M82" s="58" t="s">
+      <c r="M82" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="N82" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-20','LS11 5TP'),</v>
-      </c>
+      <c r="N82" s="25"/>
       <c r="O82" s="25"/>
-      <c r="P82" s="25"/>
-      <c r="Q82" s="25"/>
+      <c r="P82" s="25" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q82" s="32" t="s">
+        <v>457</v>
+      </c>
       <c r="R82" s="25"/>
       <c r="S82" s="25"/>
       <c r="T82" s="25"/>
@@ -11388,19 +11434,20 @@
       <c r="I83" s="25"/>
       <c r="J83" s="25"/>
       <c r="K83" s="25"/>
-      <c r="L83" s="57" t="s">
+      <c r="L83" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="M83" s="58" t="s">
+      <c r="M83" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="N83" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>('PST-21','CF10 5AE'),</v>
-      </c>
+      <c r="N83" s="25"/>
       <c r="O83" s="25"/>
-      <c r="P83" s="25"/>
-      <c r="Q83" s="25"/>
+      <c r="P83" s="25" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q83" s="32" t="s">
+        <v>459</v>
+      </c>
       <c r="R83" s="25"/>
       <c r="S83" s="25"/>
       <c r="T83" s="25"/>
@@ -11423,12 +11470,16 @@
       <c r="I84" s="25"/>
       <c r="J84" s="25"/>
       <c r="K84" s="25"/>
-      <c r="L84" s="61"/>
-      <c r="M84" s="62"/>
+      <c r="L84" s="63"/>
+      <c r="M84" s="64"/>
       <c r="N84" s="25"/>
       <c r="O84" s="25"/>
-      <c r="P84" s="25"/>
-      <c r="Q84" s="25"/>
+      <c r="P84" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="Q84" s="32" t="s">
+        <v>461</v>
+      </c>
       <c r="R84" s="25"/>
       <c r="S84" s="25"/>
       <c r="T84" s="25"/>
@@ -11441,7 +11492,7 @@
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="20" t="s">
-        <v>435</v>
+        <v>462</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="3"/>
@@ -11454,11 +11505,15 @@
       <c r="J85" s="25"/>
       <c r="K85" s="25"/>
       <c r="L85" s="25"/>
-      <c r="M85" s="32"/>
+      <c r="M85" s="33"/>
       <c r="N85" s="25"/>
       <c r="O85" s="25"/>
-      <c r="P85" s="25"/>
-      <c r="Q85" s="25"/>
+      <c r="P85" s="61" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q85" s="39" t="s">
+        <v>464</v>
+      </c>
       <c r="R85" s="25"/>
       <c r="S85" s="25"/>
       <c r="T85" s="25"/>
@@ -11482,7 +11537,7 @@
       <c r="J86" s="25"/>
       <c r="K86" s="25"/>
       <c r="L86" s="25"/>
-      <c r="M86" s="36"/>
+      <c r="M86" s="37"/>
       <c r="N86" s="25"/>
       <c r="O86" s="25"/>
       <c r="P86" s="25"/>
@@ -11499,47 +11554,53 @@
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>436</v>
+        <v>465</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>342</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>437</v>
+        <v>466</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>207</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>438</v>
+        <v>467</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>439</v>
+        <v>468</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>440</v>
+        <v>469</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>441</v>
+        <v>470</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>341</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>442</v>
+        <v>471</v>
       </c>
       <c r="K87" s="5" t="s">
         <v>245</v>
       </c>
       <c r="L87" s="5" t="s">
-        <v>443</v>
+        <v>472</v>
       </c>
       <c r="M87" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="N87" s="25"/>
-      <c r="O87" s="25"/>
-      <c r="P87" s="25"/>
+        <v>473</v>
+      </c>
+      <c r="N87" s="26" t="s">
+        <v>474</v>
+      </c>
+      <c r="O87" s="26" t="s">
+        <v>475</v>
+      </c>
+      <c r="P87" s="26" t="s">
+        <v>476</v>
+      </c>
       <c r="Q87" s="25"/>
       <c r="R87" s="25"/>
       <c r="S87" s="25"/>
@@ -11552,48 +11613,57 @@
       <c r="Z87" s="25"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="31" t="s">
-        <v>445</v>
-      </c>
-      <c r="B88" s="32" t="s">
+      <c r="A88" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="B88" s="33" t="s">
         <v>217</v>
       </c>
       <c r="C88" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D88" s="32" t="s">
+      <c r="D88" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E88" s="32" t="s">
+      <c r="E88" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="F88" s="32" t="s">
-        <v>387</v>
-      </c>
-      <c r="G88" s="32" t="s">
+      <c r="F88" s="33" t="s">
+        <v>389</v>
+      </c>
+      <c r="G88" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="H88" s="32" t="s">
+      <c r="H88" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="I88" s="32" t="s">
+      <c r="I88" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J88" s="32" t="s">
+      <c r="J88" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K88" s="32" t="s">
+      <c r="K88" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L88" s="32" t="s">
+      <c r="L88" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M88" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="N88" s="25"/>
-      <c r="O88" s="25"/>
-      <c r="P88" s="25"/>
+        <v>397</v>
+      </c>
+      <c r="N88" s="25" t="str">
+        <f t="shared" ref="N88:N104" si="3">lower(LEFT(D88,1)&amp;LOWER(TRIM(MID(D88,SEARCH(" ",D88),LEN(D88)))))&amp;1</f>
+        <v>osmith1</v>
+      </c>
+      <c r="O88" s="26">
+        <f t="shared" ref="O88:O104" si="4">RANDBETWEEN(100000,100000000)</f>
+        <v>34207961</v>
+      </c>
+      <c r="P88" s="25" t="str">
+        <f t="shared" ref="P88:P104" si="5">TEXT(today()-RANDBETWEEN(5,90),"yyyy-MM-dd")</f>
+        <v>2025-09-11</v>
+      </c>
       <c r="Q88" s="25"/>
       <c r="R88" s="25"/>
       <c r="S88" s="25"/>
@@ -11606,48 +11676,57 @@
       <c r="Z88" s="25"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="31" t="s">
-        <v>446</v>
-      </c>
-      <c r="B89" s="32" t="s">
+      <c r="A89" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="B89" s="33" t="s">
         <v>221</v>
       </c>
       <c r="C89" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D89" s="32" t="s">
+      <c r="D89" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E89" s="32" t="s">
+      <c r="E89" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="F89" s="32" t="s">
-        <v>391</v>
-      </c>
-      <c r="G89" s="32" t="s">
+      <c r="F89" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="G89" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="H89" s="32" t="s">
+      <c r="H89" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="I89" s="32">
+      <c r="I89" s="33">
         <v>1.0</v>
       </c>
-      <c r="J89" s="32" t="s">
+      <c r="J89" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K89" s="32" t="s">
+      <c r="K89" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L89" s="32" t="s">
+      <c r="L89" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M89" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="N89" s="25"/>
-      <c r="O89" s="25"/>
-      <c r="P89" s="25"/>
+        <v>402</v>
+      </c>
+      <c r="N89" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>ajones1</v>
+      </c>
+      <c r="O89" s="26">
+        <f t="shared" si="4"/>
+        <v>39429270</v>
+      </c>
+      <c r="P89" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-09-11</v>
+      </c>
       <c r="Q89" s="25"/>
       <c r="R89" s="25"/>
       <c r="S89" s="25"/>
@@ -11660,48 +11739,57 @@
       <c r="Z89" s="25"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="31" t="s">
-        <v>447</v>
-      </c>
-      <c r="B90" s="32" t="s">
+      <c r="A90" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="B90" s="33" t="s">
         <v>225</v>
       </c>
       <c r="C90" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D90" s="32" t="s">
+      <c r="D90" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="E90" s="32" t="s">
+      <c r="E90" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="F90" s="32" t="s">
-        <v>395</v>
-      </c>
-      <c r="G90" s="32" t="s">
+      <c r="F90" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="G90" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="H90" s="32" t="s">
+      <c r="H90" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="I90" s="32" t="s">
+      <c r="I90" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J90" s="32" t="s">
+      <c r="J90" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K90" s="32" t="s">
+      <c r="K90" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L90" s="32" t="s">
+      <c r="L90" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M90" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="N90" s="25"/>
-      <c r="O90" s="25"/>
-      <c r="P90" s="25"/>
+        <v>397</v>
+      </c>
+      <c r="N90" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>jtaylor1</v>
+      </c>
+      <c r="O90" s="26">
+        <f t="shared" si="4"/>
+        <v>40647216</v>
+      </c>
+      <c r="P90" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-10-07</v>
+      </c>
       <c r="Q90" s="25"/>
       <c r="R90" s="25"/>
       <c r="S90" s="25"/>
@@ -11714,48 +11802,57 @@
       <c r="Z90" s="25"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="31" t="s">
-        <v>448</v>
-      </c>
-      <c r="B91" s="32" t="s">
+      <c r="A91" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="B91" s="33" t="s">
         <v>229</v>
       </c>
       <c r="C91" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D91" s="32" t="s">
+      <c r="D91" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="E91" s="32" t="s">
+      <c r="E91" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="F91" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="G91" s="32" t="s">
+      <c r="F91" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="G91" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="H91" s="32" t="s">
+      <c r="H91" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="I91" s="32" t="s">
+      <c r="I91" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J91" s="32" t="s">
+      <c r="J91" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K91" s="32" t="s">
+      <c r="K91" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L91" s="32" t="s">
+      <c r="L91" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M91" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="N91" s="25"/>
-      <c r="O91" s="25"/>
-      <c r="P91" s="25"/>
+        <v>397</v>
+      </c>
+      <c r="N91" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>obrown1</v>
+      </c>
+      <c r="O91" s="26">
+        <f t="shared" si="4"/>
+        <v>23234299</v>
+      </c>
+      <c r="P91" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-09-01</v>
+      </c>
       <c r="Q91" s="25"/>
       <c r="R91" s="25"/>
       <c r="S91" s="25"/>
@@ -11768,48 +11865,57 @@
       <c r="Z91" s="25"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="31" t="s">
-        <v>449</v>
-      </c>
-      <c r="B92" s="32" t="s">
+      <c r="A92" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B92" s="33" t="s">
         <v>233</v>
       </c>
       <c r="C92" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D92" s="32" t="s">
+      <c r="D92" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="E92" s="32" t="s">
+      <c r="E92" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="F92" s="32" t="s">
-        <v>403</v>
-      </c>
-      <c r="G92" s="32" t="s">
+      <c r="F92" s="33" t="s">
+        <v>409</v>
+      </c>
+      <c r="G92" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="H92" s="32" t="s">
+      <c r="H92" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="I92" s="32">
+      <c r="I92" s="33">
         <v>2.0</v>
       </c>
-      <c r="J92" s="32" t="s">
+      <c r="J92" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K92" s="32" t="s">
+      <c r="K92" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L92" s="32" t="s">
+      <c r="L92" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M92" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="N92" s="25"/>
-      <c r="O92" s="25"/>
-      <c r="P92" s="25"/>
+        <v>402</v>
+      </c>
+      <c r="N92" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>hwilson1</v>
+      </c>
+      <c r="O92" s="26">
+        <f t="shared" si="4"/>
+        <v>89068681</v>
+      </c>
+      <c r="P92" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-09-23</v>
+      </c>
       <c r="Q92" s="25"/>
       <c r="R92" s="25"/>
       <c r="S92" s="25"/>
@@ -11822,48 +11928,57 @@
       <c r="Z92" s="25"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="31" t="s">
-        <v>450</v>
-      </c>
-      <c r="B93" s="32" t="s">
+      <c r="A93" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="B93" s="33" t="s">
         <v>235</v>
       </c>
       <c r="C93" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D93" s="32" t="s">
+      <c r="D93" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="E93" s="32" t="s">
+      <c r="E93" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="F93" s="32" t="s">
-        <v>405</v>
-      </c>
-      <c r="G93" s="32" t="s">
+      <c r="F93" s="33" t="s">
+        <v>412</v>
+      </c>
+      <c r="G93" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="H93" s="32" t="s">
+      <c r="H93" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="I93" s="32" t="s">
+      <c r="I93" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J93" s="32" t="s">
+      <c r="J93" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K93" s="32" t="s">
+      <c r="K93" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L93" s="32" t="s">
+      <c r="L93" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M93" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="N93" s="25"/>
-      <c r="O93" s="25"/>
-      <c r="P93" s="25"/>
+        <v>397</v>
+      </c>
+      <c r="N93" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>ithompson1</v>
+      </c>
+      <c r="O93" s="26">
+        <f t="shared" si="4"/>
+        <v>76552312</v>
+      </c>
+      <c r="P93" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-10-11</v>
+      </c>
       <c r="Q93" s="25"/>
       <c r="R93" s="25"/>
       <c r="S93" s="25"/>
@@ -11876,48 +11991,57 @@
       <c r="Z93" s="25"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="31" t="s">
-        <v>451</v>
-      </c>
-      <c r="B94" s="32" t="s">
+      <c r="A94" s="32" t="s">
+        <v>416</v>
+      </c>
+      <c r="B94" s="33" t="s">
         <v>237</v>
       </c>
       <c r="C94" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D94" s="32" t="s">
+      <c r="D94" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="E94" s="32" t="s">
+      <c r="E94" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="F94" s="32" t="s">
-        <v>407</v>
-      </c>
-      <c r="G94" s="32" t="s">
+      <c r="F94" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="G94" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="H94" s="32" t="s">
+      <c r="H94" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="I94" s="32" t="s">
+      <c r="I94" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J94" s="32" t="s">
+      <c r="J94" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K94" s="32" t="s">
+      <c r="K94" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L94" s="32" t="s">
+      <c r="L94" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M94" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="N94" s="25"/>
-      <c r="O94" s="25"/>
-      <c r="P94" s="25"/>
+        <v>397</v>
+      </c>
+      <c r="N94" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>cjohnson1</v>
+      </c>
+      <c r="O94" s="26">
+        <f t="shared" si="4"/>
+        <v>68279697</v>
+      </c>
+      <c r="P94" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-09-10</v>
+      </c>
       <c r="Q94" s="25"/>
       <c r="R94" s="25"/>
       <c r="S94" s="25"/>
@@ -11930,48 +12054,57 @@
       <c r="Z94" s="25"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="31" t="s">
-        <v>452</v>
-      </c>
-      <c r="B95" s="32" t="s">
+      <c r="A95" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="B95" s="33" t="s">
         <v>239</v>
       </c>
       <c r="C95" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D95" s="32" t="s">
+      <c r="D95" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="E95" s="32" t="s">
+      <c r="E95" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="F95" s="32" t="s">
-        <v>409</v>
-      </c>
-      <c r="G95" s="32" t="s">
+      <c r="F95" s="33" t="s">
+        <v>418</v>
+      </c>
+      <c r="G95" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="H95" s="32" t="s">
+      <c r="H95" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="I95" s="32" t="s">
+      <c r="I95" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J95" s="32" t="s">
+      <c r="J95" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K95" s="32" t="s">
+      <c r="K95" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L95" s="32" t="s">
+      <c r="L95" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M95" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="N95" s="25"/>
-      <c r="O95" s="25"/>
-      <c r="P95" s="25"/>
+        <v>397</v>
+      </c>
+      <c r="N95" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>ewalker1</v>
+      </c>
+      <c r="O95" s="26">
+        <f t="shared" si="4"/>
+        <v>2975614</v>
+      </c>
+      <c r="P95" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-09-07</v>
+      </c>
       <c r="Q95" s="25"/>
       <c r="R95" s="25"/>
       <c r="S95" s="25"/>
@@ -11984,48 +12117,57 @@
       <c r="Z95" s="25"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="31" t="s">
-        <v>453</v>
-      </c>
-      <c r="B96" s="32" t="s">
+      <c r="A96" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="B96" s="33" t="s">
         <v>241</v>
       </c>
       <c r="C96" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D96" s="32" t="s">
+      <c r="D96" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="E96" s="32" t="s">
+      <c r="E96" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="F96" s="32" t="s">
-        <v>411</v>
-      </c>
-      <c r="G96" s="32" t="s">
+      <c r="F96" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="G96" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="H96" s="32" t="s">
+      <c r="H96" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="I96" s="32" t="s">
+      <c r="I96" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J96" s="32" t="s">
+      <c r="J96" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K96" s="32" t="s">
+      <c r="K96" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L96" s="32" t="s">
+      <c r="L96" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M96" s="21" t="s">
-        <v>393</v>
-      </c>
-      <c r="N96" s="25"/>
-      <c r="O96" s="25"/>
-      <c r="P96" s="25"/>
+        <v>397</v>
+      </c>
+      <c r="N96" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>gevans1</v>
+      </c>
+      <c r="O96" s="26">
+        <f t="shared" si="4"/>
+        <v>24679679</v>
+      </c>
+      <c r="P96" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-10-12</v>
+      </c>
       <c r="Q96" s="25"/>
       <c r="R96" s="25"/>
       <c r="S96" s="25"/>
@@ -12038,48 +12180,57 @@
       <c r="Z96" s="25"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="31" t="s">
-        <v>454</v>
-      </c>
-      <c r="B97" s="32" t="s">
+      <c r="A97" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="B97" s="33" t="s">
         <v>243</v>
       </c>
       <c r="C97" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D97" s="32" t="s">
+      <c r="D97" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="E97" s="32" t="s">
+      <c r="E97" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="F97" s="32" t="s">
-        <v>413</v>
-      </c>
-      <c r="G97" s="32" t="s">
+      <c r="F97" s="33" t="s">
+        <v>424</v>
+      </c>
+      <c r="G97" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="H97" s="32" t="s">
+      <c r="H97" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="I97" s="32">
+      <c r="I97" s="33">
         <v>3.0</v>
       </c>
-      <c r="J97" s="32" t="s">
+      <c r="J97" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="K97" s="32" t="s">
+      <c r="K97" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="L97" s="32" t="s">
+      <c r="L97" s="33" t="s">
         <v>46</v>
       </c>
       <c r="M97" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="N97" s="25"/>
-      <c r="O97" s="25"/>
-      <c r="P97" s="25"/>
+        <v>402</v>
+      </c>
+      <c r="N97" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>arobinson1</v>
+      </c>
+      <c r="O97" s="26">
+        <f t="shared" si="4"/>
+        <v>64155041</v>
+      </c>
+      <c r="P97" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-09-02</v>
+      </c>
       <c r="Q97" s="25"/>
       <c r="R97" s="25"/>
       <c r="S97" s="25"/>
@@ -12092,49 +12243,58 @@
       <c r="Z97" s="25"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="31" t="s">
-        <v>455</v>
-      </c>
-      <c r="B98" s="32" t="s">
+      <c r="A98" s="32" t="s">
+        <v>451</v>
+      </c>
+      <c r="B98" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C98" s="25" t="s">
-        <v>456</v>
-      </c>
-      <c r="D98" s="32" t="s">
+        <v>450</v>
+      </c>
+      <c r="D98" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E98" s="32" t="s">
-        <v>457</v>
-      </c>
-      <c r="F98" s="32" t="s">
-        <v>415</v>
-      </c>
-      <c r="G98" s="32" t="str">
-        <f t="shared" ref="G98:G104" si="4">SUBSTITUTE(D98," ",".")&amp;"@email.com"</f>
+      <c r="E98" s="33" t="s">
+        <v>477</v>
+      </c>
+      <c r="F98" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="G98" s="33" t="str">
+        <f t="shared" ref="G98:G104" si="6">SUBSTITUTE(D98," ",".")&amp;"@email.com"</f>
         <v>Simon.Lee@email.com</v>
       </c>
-      <c r="H98" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="I98" s="32" t="s">
+      <c r="H98" s="33" t="s">
+        <v>478</v>
+      </c>
+      <c r="I98" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="J98" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="K98" s="32" t="s">
+      <c r="J98" s="33" t="s">
+        <v>479</v>
+      </c>
+      <c r="K98" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="L98" s="32">
+      <c r="L98" s="33">
         <v>2.0</v>
       </c>
       <c r="M98" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="N98" s="25"/>
-      <c r="O98" s="25"/>
-      <c r="P98" s="25"/>
+        <v>407</v>
+      </c>
+      <c r="N98" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>slee1</v>
+      </c>
+      <c r="O98" s="26">
+        <f t="shared" si="4"/>
+        <v>23786402</v>
+      </c>
+      <c r="P98" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-10-29</v>
+      </c>
       <c r="Q98" s="25"/>
       <c r="R98" s="25"/>
       <c r="S98" s="25"/>
@@ -12147,49 +12307,58 @@
       <c r="Z98" s="25"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="31" t="s">
-        <v>460</v>
-      </c>
-      <c r="B99" s="32" t="s">
+      <c r="A99" s="32" t="s">
+        <v>453</v>
+      </c>
+      <c r="B99" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C99" s="25" t="s">
-        <v>461</v>
-      </c>
-      <c r="D99" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="D99" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="E99" s="32" t="s">
-        <v>462</v>
-      </c>
-      <c r="F99" s="32" t="s">
-        <v>418</v>
-      </c>
-      <c r="G99" s="32" t="str">
+      <c r="E99" s="33" t="s">
+        <v>480</v>
+      </c>
+      <c r="F99" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="G99" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v>Jen.Keeosk@email.com</v>
+      </c>
+      <c r="H99" s="33" t="s">
+        <v>481</v>
+      </c>
+      <c r="I99" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J99" s="33" t="s">
+        <v>479</v>
+      </c>
+      <c r="K99" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="L99" s="33">
+        <v>3.0</v>
+      </c>
+      <c r="M99" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="N99" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>jkeeosk1</v>
+      </c>
+      <c r="O99" s="26">
         <f t="shared" si="4"/>
-        <v>Jen.Keeosk@email.com</v>
-      </c>
-      <c r="H99" s="32" t="s">
-        <v>463</v>
-      </c>
-      <c r="I99" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="J99" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="K99" s="32" t="s">
-        <v>254</v>
-      </c>
-      <c r="L99" s="32">
-        <v>3.0</v>
-      </c>
-      <c r="M99" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="N99" s="25"/>
-      <c r="O99" s="25"/>
-      <c r="P99" s="25"/>
+        <v>16254758</v>
+      </c>
+      <c r="P99" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-11-14</v>
+      </c>
       <c r="Q99" s="25"/>
       <c r="R99" s="25"/>
       <c r="S99" s="25"/>
@@ -12202,49 +12371,58 @@
       <c r="Z99" s="25"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="31" t="s">
-        <v>464</v>
-      </c>
-      <c r="B100" s="32" t="s">
+      <c r="A100" s="32" t="s">
+        <v>455</v>
+      </c>
+      <c r="B100" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C100" s="25" t="s">
-        <v>465</v>
-      </c>
-      <c r="D100" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D100" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E100" s="32" t="s">
-        <v>466</v>
-      </c>
-      <c r="F100" s="32" t="s">
-        <v>421</v>
-      </c>
-      <c r="G100" s="32" t="str">
+      <c r="E100" s="33" t="s">
+        <v>482</v>
+      </c>
+      <c r="F100" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="G100" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v>Jason.Anderson@email.com</v>
+      </c>
+      <c r="H100" s="33" t="s">
+        <v>483</v>
+      </c>
+      <c r="I100" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J100" s="33" t="s">
+        <v>479</v>
+      </c>
+      <c r="K100" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="L100" s="33">
+        <v>2.0</v>
+      </c>
+      <c r="M100" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="N100" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>janderson1</v>
+      </c>
+      <c r="O100" s="26">
         <f t="shared" si="4"/>
-        <v>Jason.Anderson@email.com</v>
-      </c>
-      <c r="H100" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="I100" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="J100" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="K100" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="L100" s="32">
-        <v>2.0</v>
-      </c>
-      <c r="M100" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="N100" s="25"/>
-      <c r="O100" s="25"/>
-      <c r="P100" s="25"/>
+        <v>48894360</v>
+      </c>
+      <c r="P100" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-09-28</v>
+      </c>
       <c r="Q100" s="25"/>
       <c r="R100" s="25"/>
       <c r="S100" s="25"/>
@@ -12257,49 +12435,58 @@
       <c r="Z100" s="25"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="31" t="s">
-        <v>468</v>
-      </c>
-      <c r="B101" s="32" t="s">
+      <c r="A101" s="32" t="s">
+        <v>457</v>
+      </c>
+      <c r="B101" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C101" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="D101" s="32" t="s">
+        <v>456</v>
+      </c>
+      <c r="D101" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="E101" s="32" t="s">
-        <v>470</v>
-      </c>
-      <c r="F101" s="32" t="s">
-        <v>424</v>
-      </c>
-      <c r="G101" s="32" t="str">
+      <c r="E101" s="33" t="s">
+        <v>484</v>
+      </c>
+      <c r="F101" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="G101" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v>Jim.Bean@email.com</v>
+      </c>
+      <c r="H101" s="33" t="s">
+        <v>485</v>
+      </c>
+      <c r="I101" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J101" s="33" t="s">
+        <v>479</v>
+      </c>
+      <c r="K101" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="L101" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="M101" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="N101" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>jbean1</v>
+      </c>
+      <c r="O101" s="26">
         <f t="shared" si="4"/>
-        <v>Jim.Bean@email.com</v>
-      </c>
-      <c r="H101" s="32" t="s">
-        <v>471</v>
-      </c>
-      <c r="I101" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="J101" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="K101" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="L101" s="32">
-        <v>4.0</v>
-      </c>
-      <c r="M101" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="N101" s="25"/>
-      <c r="O101" s="25"/>
-      <c r="P101" s="25"/>
+        <v>47365148</v>
+      </c>
+      <c r="P101" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-09-21</v>
+      </c>
       <c r="Q101" s="25"/>
       <c r="R101" s="25"/>
       <c r="S101" s="25"/>
@@ -12312,49 +12499,58 @@
       <c r="Z101" s="25"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="31" t="s">
-        <v>472</v>
-      </c>
-      <c r="B102" s="32" t="s">
+      <c r="A102" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="B102" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C102" s="25" t="s">
-        <v>473</v>
-      </c>
-      <c r="D102" s="32" t="s">
+        <v>458</v>
+      </c>
+      <c r="D102" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E102" s="32" t="s">
-        <v>474</v>
-      </c>
-      <c r="F102" s="32" t="s">
-        <v>427</v>
-      </c>
-      <c r="G102" s="32" t="str">
+      <c r="E102" s="33" t="s">
+        <v>486</v>
+      </c>
+      <c r="F102" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="G102" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v>Katie.John@email.com</v>
+      </c>
+      <c r="H102" s="33" t="s">
+        <v>487</v>
+      </c>
+      <c r="I102" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J102" s="33" t="s">
+        <v>479</v>
+      </c>
+      <c r="K102" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="L102" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="M102" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="N102" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>kjohn1</v>
+      </c>
+      <c r="O102" s="26">
         <f t="shared" si="4"/>
-        <v>Katie.John@email.com</v>
-      </c>
-      <c r="H102" s="32" t="s">
-        <v>475</v>
-      </c>
-      <c r="I102" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="J102" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="K102" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="L102" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="M102" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="N102" s="25"/>
-      <c r="O102" s="25"/>
-      <c r="P102" s="25"/>
+        <v>46012405</v>
+      </c>
+      <c r="P102" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-11-04</v>
+      </c>
       <c r="Q102" s="25"/>
       <c r="R102" s="25"/>
       <c r="S102" s="25"/>
@@ -12367,49 +12563,58 @@
       <c r="Z102" s="25"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="31" t="s">
-        <v>476</v>
-      </c>
-      <c r="B103" s="32" t="s">
+      <c r="A103" s="32" t="s">
+        <v>461</v>
+      </c>
+      <c r="B103" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C103" s="25" t="s">
-        <v>477</v>
-      </c>
-      <c r="D103" s="32" t="s">
-        <v>478</v>
-      </c>
-      <c r="E103" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="F103" s="32" t="s">
-        <v>430</v>
-      </c>
-      <c r="G103" s="32" t="str">
+        <v>460</v>
+      </c>
+      <c r="D103" s="33" t="s">
+        <v>488</v>
+      </c>
+      <c r="E103" s="33" t="s">
+        <v>489</v>
+      </c>
+      <c r="F103" s="33" t="s">
+        <v>443</v>
+      </c>
+      <c r="G103" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v>Sue.Bridges@email.com</v>
+      </c>
+      <c r="H103" s="33" t="s">
+        <v>490</v>
+      </c>
+      <c r="I103" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J103" s="33" t="s">
+        <v>491</v>
+      </c>
+      <c r="K103" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="L103" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="M103" s="34" t="s">
+        <v>392</v>
+      </c>
+      <c r="N103" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>sbridges1</v>
+      </c>
+      <c r="O103" s="26">
         <f t="shared" si="4"/>
-        <v>Sue.Bridges@email.com</v>
-      </c>
-      <c r="H103" s="32" t="s">
-        <v>480</v>
-      </c>
-      <c r="I103" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="J103" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="K103" s="32" t="s">
-        <v>482</v>
-      </c>
-      <c r="L103" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="M103" s="33" t="s">
-        <v>389</v>
-      </c>
-      <c r="N103" s="25"/>
-      <c r="O103" s="25"/>
-      <c r="P103" s="25"/>
+        <v>37980214</v>
+      </c>
+      <c r="P103" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-11-06</v>
+      </c>
       <c r="Q103" s="25"/>
       <c r="R103" s="25"/>
       <c r="S103" s="25"/>
@@ -12422,49 +12627,58 @@
       <c r="Z103" s="25"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="B104" s="36" t="s">
+      <c r="A104" s="39" t="s">
+        <v>464</v>
+      </c>
+      <c r="B104" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C104" s="59" t="s">
-        <v>484</v>
-      </c>
-      <c r="D104" s="36" t="s">
-        <v>485</v>
-      </c>
-      <c r="E104" s="36" t="s">
-        <v>486</v>
-      </c>
-      <c r="F104" s="36" t="s">
-        <v>433</v>
-      </c>
-      <c r="G104" s="36" t="str">
+      <c r="C104" s="61" t="s">
+        <v>463</v>
+      </c>
+      <c r="D104" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="E104" s="37" t="s">
+        <v>494</v>
+      </c>
+      <c r="F104" s="37" t="s">
+        <v>448</v>
+      </c>
+      <c r="G104" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v>Alex.Towns@email.com</v>
+      </c>
+      <c r="H104" s="37" t="s">
+        <v>495</v>
+      </c>
+      <c r="I104" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="J104" s="37" t="s">
+        <v>491</v>
+      </c>
+      <c r="K104" s="37" t="s">
+        <v>496</v>
+      </c>
+      <c r="L104" s="37">
+        <v>2.0</v>
+      </c>
+      <c r="M104" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="N104" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>atowns1</v>
+      </c>
+      <c r="O104" s="26">
         <f t="shared" si="4"/>
-        <v>Alex.Towns@email.com</v>
-      </c>
-      <c r="H104" s="36" t="s">
-        <v>487</v>
-      </c>
-      <c r="I104" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="J104" s="36" t="s">
-        <v>481</v>
-      </c>
-      <c r="K104" s="36" t="s">
-        <v>488</v>
-      </c>
-      <c r="L104" s="36">
-        <v>2.0</v>
-      </c>
-      <c r="M104" s="37" t="s">
-        <v>389</v>
-      </c>
-      <c r="N104" s="25"/>
-      <c r="O104" s="25"/>
-      <c r="P104" s="25"/>
+        <v>33917371</v>
+      </c>
+      <c r="P104" s="25" t="str">
+        <f t="shared" si="5"/>
+        <v>2025-08-26</v>
+      </c>
       <c r="Q104" s="25"/>
       <c r="R104" s="25"/>
       <c r="S104" s="25"/>

</xml_diff>